<commit_message>
Development updates, changed prefix from BE to SA
</commit_message>
<xml_diff>
--- a/Processes/SA_EnrollDrop/Data/Config.xlsx
+++ b/Processes/SA_EnrollDrop/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Desktop\UQ Add-Drop Enrollments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D3DF938-47AA-4654-A692-1EE059D93273}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89D911BE-2193-482B-8C10-8D5118165A3E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31860" yWindow="1095" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4830" yWindow="1965" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -165,24 +165,15 @@
     <t>This is a logging field which allows you to group the log data of two or more subprocesses under the same business process name</t>
   </si>
   <si>
-    <t>BE_Sinet_URL</t>
-  </si>
-  <si>
     <t>SI-net URL</t>
   </si>
   <si>
     <t>Sinet_URL</t>
   </si>
   <si>
-    <t>BE_Enroll-Drop</t>
-  </si>
-  <si>
     <t>OrchestratorQueueName</t>
   </si>
   <si>
-    <t>BE_Sinet_ErrorEmailAddress</t>
-  </si>
-  <si>
     <t>Email address for error emails</t>
   </si>
   <si>
@@ -201,31 +192,40 @@
     <t>SMTP Server Address</t>
   </si>
   <si>
-    <t>BE_Sinet_InputFileName</t>
-  </si>
-  <si>
     <t>InputFileName</t>
   </si>
   <si>
     <t>Input file of class adds and drops</t>
   </si>
   <si>
-    <t>BE_Sinet_InputFileSheetName</t>
-  </si>
-  <si>
     <t>Input file sheet name</t>
   </si>
   <si>
     <t>InputFileSheetName</t>
   </si>
   <si>
-    <t>BE_Sinet_InputFilePath</t>
-  </si>
-  <si>
     <t>Input file sheet path</t>
   </si>
   <si>
     <t>InputFilePath</t>
+  </si>
+  <si>
+    <t>SA_Sinet_URL</t>
+  </si>
+  <si>
+    <t>SA_Sinet_ErrorEmailAddress</t>
+  </si>
+  <si>
+    <t>SA_Sinet_InputFileName</t>
+  </si>
+  <si>
+    <t>SA_Sinet_InputFileSheetName</t>
+  </si>
+  <si>
+    <t>SA_Sinet_InputFilePath</t>
+  </si>
+  <si>
+    <t>SA_Enroll-Drop</t>
   </si>
 </sst>
 </file>
@@ -632,10 +632,10 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B2" t="s">
-        <v>50</v>
+        <v>67</v>
       </c>
       <c r="C2" t="s">
         <v>43</v>
@@ -1655,7 +1655,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2867,8 +2867,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2912,79 +2912,79 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" t="s">
         <v>47</v>
-      </c>
-      <c r="C2" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B3" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="C3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B5" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C5" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B6" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="C6" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B7" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="C7" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="B8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C8" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Renamed assets to "SA_EnrollDrop_*", mapping of network share using SSO account
</commit_message>
<xml_diff>
--- a/Processes/SA_EnrollDrop/Data/Config.xlsx
+++ b/Processes/SA_EnrollDrop/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Desktop\UQ Add-Drop Enrollments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89D911BE-2193-482B-8C10-8D5118165A3E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A40CE001-5627-40B5-8C70-00F42EC219E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4830" yWindow="1965" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5040" yWindow="1995" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -210,22 +210,22 @@
     <t>InputFilePath</t>
   </si>
   <si>
-    <t>SA_Sinet_URL</t>
-  </si>
-  <si>
-    <t>SA_Sinet_ErrorEmailAddress</t>
-  </si>
-  <si>
-    <t>SA_Sinet_InputFileName</t>
-  </si>
-  <si>
-    <t>SA_Sinet_InputFileSheetName</t>
-  </si>
-  <si>
-    <t>SA_Sinet_InputFilePath</t>
-  </si>
-  <si>
     <t>SA_Enroll-Drop</t>
+  </si>
+  <si>
+    <t>SA_EnrollDrop_Sinet_URL</t>
+  </si>
+  <si>
+    <t>SA_EnrollDrop_ErrorEmailAddress</t>
+  </si>
+  <si>
+    <t>SA_EnrollDrop_InputFileName</t>
+  </si>
+  <si>
+    <t>SA_EnrollDrop_InputFilePath</t>
+  </si>
+  <si>
+    <t>SA_EnrollDrop_InputFileSheetName</t>
   </si>
 </sst>
 </file>
@@ -265,9 +265,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -635,7 +636,7 @@
         <v>49</v>
       </c>
       <c r="B2" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="C2" t="s">
         <v>43</v>
@@ -1655,7 +1656,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2867,8 +2868,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2914,8 +2915,8 @@
       <c r="A2" t="s">
         <v>48</v>
       </c>
-      <c r="B2" t="s">
-        <v>62</v>
+      <c r="B2" s="2" t="s">
+        <v>63</v>
       </c>
       <c r="C2" t="s">
         <v>47</v>
@@ -2925,8 +2926,8 @@
       <c r="A3" t="s">
         <v>51</v>
       </c>
-      <c r="B3" t="s">
-        <v>63</v>
+      <c r="B3" s="2" t="s">
+        <v>64</v>
       </c>
       <c r="C3" t="s">
         <v>50</v>
@@ -2958,8 +2959,8 @@
       <c r="A6" t="s">
         <v>56</v>
       </c>
-      <c r="B6" t="s">
-        <v>64</v>
+      <c r="B6" s="2" t="s">
+        <v>65</v>
       </c>
       <c r="C6" t="s">
         <v>57</v>
@@ -2969,8 +2970,8 @@
       <c r="A7" t="s">
         <v>59</v>
       </c>
-      <c r="B7" t="s">
-        <v>65</v>
+      <c r="B7" s="2" t="s">
+        <v>67</v>
       </c>
       <c r="C7" t="s">
         <v>58</v>
@@ -2980,7 +2981,7 @@
       <c r="A8" t="s">
         <v>61</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="2" t="s">
         <v>66</v>
       </c>
       <c r="C8" t="s">

</xml_diff>